<commit_message>
days and hours:: by sergio giraldo @ 20230306T1059CET, gpg signed
</commit_message>
<xml_diff>
--- a/excel/validation.xlsx
+++ b/excel/validation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GK47LX/source/office/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5E94B2-1A42-4B44-93E7-1F30EE95D950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174B63FE-A7FD-FB43-9238-EB2BF241A825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20440" activeTab="1" xr2:uid="{11F90907-D0F3-EE49-8B50-E4314E23B54D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>people</t>
   </si>
@@ -196,6 +196,12 @@
     </r>
   </si>
   <si>
+    <t>br34</t>
+  </si>
+  <si>
+    <t>s1234</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">0. Must be 'XXX' or 2 numbers
 </t>
@@ -208,15 +214,10 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">1. Custom validation as columns C and D
-</t>
+      <t>1. Custom validation as columns C and D
+2. Using formula 
+=OR(E4="XXX";AND(LEN(E4)= 2; ISNUMBER(E4)))</t>
     </r>
-  </si>
-  <si>
-    <t>br34</t>
-  </si>
-  <si>
-    <t>s1234</t>
   </si>
 </sst>
 </file>
@@ -839,7 +840,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -866,7 +867,7 @@
         <v>20</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -899,7 +900,9 @@
       <c r="D3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -996,7 +999,7 @@
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E16" s="5"/>
     </row>
@@ -1004,7 +1007,7 @@
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>

</xml_diff>